<commit_message>
third commit added feeds pages
</commit_message>
<xml_diff>
--- a/Excel/Testdatap.xlsx
+++ b/Excel/Testdatap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PageObjectModell\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1507F7-BC33-4705-A5D0-61A6F5680DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4374B415-11E4-438A-A54F-BA732053C55D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>TC</t>
   </si>
@@ -70,6 +70,9 @@
   <si>
     <t>This field acts as a calculator for any expression you input.
 E.g. 20+20 will yield 40 automatically</t>
+  </si>
+  <si>
+    <t>Rayat</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBF5AE0-28E2-466F-8104-BAB314B4CBD1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,6 +457,14 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>